<commit_message>
Allow correlating discrete variables
</commit_message>
<xml_diff>
--- a/tests/sensitivities/data/config/design_input_mc_with_correls.xlsx
+++ b/tests/sensitivities/data/config/design_input_mc_with_correls.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statoilsrm-my.sharepoint.com/personal/tral_equinor_com/Documents/FMU_stdmat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52AC414D-7111-4FD5-9841-A07DB1ED395D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EC186C-3D14-DE49-BDBF-460B38239368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="23580" windowHeight="13605" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26280" yWindow="2660" windowWidth="30740" windowHeight="17940" tabRatio="990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
     <sheet name="designinput" sheetId="2" r:id="rId2"/>
     <sheet name="corr1" sheetId="3" r:id="rId3"/>
     <sheet name="corr2" sheetId="4" r:id="rId4"/>
-    <sheet name="depend1" sheetId="5" r:id="rId5"/>
-    <sheet name="defaultvalues" sheetId="6" r:id="rId6"/>
-    <sheet name="INFO" sheetId="7" r:id="rId7"/>
+    <sheet name="corr3" sheetId="8" r:id="rId5"/>
+    <sheet name="depend1" sheetId="5" r:id="rId6"/>
+    <sheet name="defaultvalues" sheetId="6" r:id="rId7"/>
+    <sheet name="INFO" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports">0</definedName>
@@ -198,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>designtype</t>
   </si>
@@ -420,6 +421,9 @@
   </si>
   <si>
     <t>oocalc filename.xlsx</t>
+  </si>
+  <si>
+    <t>corr3</t>
   </si>
 </sst>
 </file>
@@ -549,17 +553,14 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -570,38 +571,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -611,7 +606,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1004,9 +999,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1044,7 +1039,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1150,7 +1145,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1292,7 +1287,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1302,19 +1297,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375"/>
+    <col min="1" max="1" width="14.6640625"/>
     <col min="2" max="2" width="10"/>
-    <col min="3" max="3" width="77.85546875"/>
-    <col min="4" max="1025" width="8.7109375"/>
+    <col min="3" max="3" width="77.83203125"/>
+    <col min="4" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1363,403 +1358,407 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D9" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3"/>
-    <col min="2" max="2" width="8.28515625" style="4"/>
-    <col min="3" max="3" width="5.42578125" style="4"/>
-    <col min="4" max="4" width="12" style="4"/>
-    <col min="5" max="5" width="9.5703125" style="2"/>
-    <col min="6" max="6" width="6.85546875" style="2"/>
-    <col min="7" max="7" width="9.5703125" style="2"/>
-    <col min="8" max="8" width="6.85546875" style="2"/>
-    <col min="9" max="9" width="9.85546875" style="4"/>
-    <col min="10" max="10" width="31.42578125" style="2"/>
-    <col min="11" max="13" width="11.28515625" style="2"/>
-    <col min="14" max="14" width="8.85546875" style="2"/>
-    <col min="15" max="15" width="10" style="4"/>
-    <col min="16" max="16" width="10.28515625" style="4"/>
-    <col min="17" max="17" width="12.7109375"/>
-    <col min="18" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="10.6640625" style="3"/>
+    <col min="2" max="2" width="8.33203125" style="2"/>
+    <col min="3" max="3" width="5.5" style="2"/>
+    <col min="4" max="4" width="12" style="2"/>
+    <col min="5" max="5" width="9.5" style="2"/>
+    <col min="6" max="6" width="6.83203125" style="2"/>
+    <col min="7" max="7" width="9.5" style="2"/>
+    <col min="8" max="8" width="6.83203125" style="2"/>
+    <col min="9" max="9" width="9.83203125" style="2"/>
+    <col min="10" max="10" width="31.5" style="2"/>
+    <col min="11" max="13" width="11.33203125" style="2"/>
+    <col min="14" max="14" width="8.83203125" style="2"/>
+    <col min="15" max="15" width="10" style="2"/>
+    <col min="16" max="16" width="10.33203125" style="2"/>
+    <col min="17" max="17" width="12.6640625"/>
+    <col min="18" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="Q1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>500</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="8">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8">
+      <c r="M2" s="8"/>
+      <c r="N2" s="7">
         <v>3</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>0</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="8">
         <v>1</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="8">
         <v>-1</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="8">
         <v>1</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <v>2</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>1</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>10</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="8">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7">
         <v>3</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>2500</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>2550</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="8">
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7">
         <v>1</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>2430</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>2470</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="8">
         <v>2500</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="8">
+      <c r="M6" s="8"/>
+      <c r="N6" s="7">
         <v>1</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>2400</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="8">
         <v>2450</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <v>2500</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="8">
+      <c r="M7" s="8"/>
+      <c r="N7" s="7">
         <v>1</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8" t="s">
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>0.75</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>0.8</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>1</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="8">
+      <c r="M9" s="8"/>
+      <c r="N9" s="7">
         <v>2</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8" t="s">
+      <c r="O9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>0.5</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>0.6</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>0.65</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="8">
+      <c r="M10" s="8"/>
+      <c r="N10" s="7">
         <v>2</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="8">
         <v>1</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="8">
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7">
         <v>3</v>
       </c>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1781,58 +1780,58 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="4"/>
-    <col min="2" max="4" width="8.5703125" style="4"/>
-    <col min="5" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="14.83203125" style="2"/>
+    <col min="2" max="4" width="8.5" style="2"/>
+    <col min="5" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>0</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>0.2</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1846,64 +1845,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="4"/>
-    <col min="2" max="2" width="18.140625" style="4"/>
-    <col min="3" max="3" width="13.85546875" style="4"/>
-    <col min="4" max="4" width="12.42578125" style="4"/>
-    <col min="5" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="14.83203125" style="2"/>
+    <col min="2" max="2" width="18.1640625" style="2"/>
+    <col min="3" max="3" width="13.83203125" style="2"/>
+    <col min="4" max="4" width="12.5" style="2"/>
+    <col min="5" max="1024" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>0.5</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>-0.7</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>-0.7</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1914,6 +1913,48 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272FB4C1-4B21-1E49-B8E2-B257F97AD1D4}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1921,14 +1962,14 @@
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
+    <col min="1" max="1" width="11.5"/>
     <col min="2" max="3" width="16"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="4" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1939,8 +1980,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B2">
@@ -1950,7 +1991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1961,7 +2002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1971,322 +2012,7 @@
       <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D56"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A15:A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" style="4"/>
-    <col min="2" max="2" width="12.140625" style="15"/>
-    <col min="3" max="999" width="8.7109375"/>
-    <col min="1000" max="1025" width="8.85546875"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="15">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="15">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="19">
-        <v>0.45</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26" s="19"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="21"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="21"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="21"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="21"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="21"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="21"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="21"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37" s="19"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38" s="19"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39" s="19"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40" s="19"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41" s="19"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42" s="19"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43" s="19"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45" s="19"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46" s="19"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47" s="19"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48" s="19"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49" s="19"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50" s="19"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51" s="19"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52" s="19"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53" s="19"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54" s="19"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55" s="19"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56" s="19"/>
+      <c r="F4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2299,43 +2025,330 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A16" sqref="A15:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.5" style="2"/>
+    <col min="2" max="2" width="12.1640625" style="14"/>
+    <col min="3" max="999" width="8.6640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="18"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="18"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="18"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="18"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="18"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="18"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="18"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -2346,7 +2359,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2369,6 +2382,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="02f74cf1-ae9f-400d-bc52-3bcd3a9e177f" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3F81C8E0C6D6E4B8B0E11E1FD2C3815" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="831350f1af26471ff20340f15875df59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="24e64fd7-dd82-45ab-bc56-7bee2b649a8c" xmlns:ns4="7518fa5f-d3e5-45ff-bc46-9421360fd0ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e9136827b31234ee1bd7613b24a8ed12" ns3:_="" ns4:_="">
     <xsd:import namespace="24e64fd7-dd82-45ab-bc56-7bee2b649a8c"/>
@@ -2571,27 +2604,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="02f74cf1-ae9f-400d-bc52-3bcd3a9e177f" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FDBEAEB-23AE-46E2-827B-BF6C7AC8C447}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7518fa5f-d3e5-45ff-bc46-9421360fd0ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="24e64fd7-dd82-45ab-bc56-7bee2b649a8c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500F210C-5797-4401-A254-1609F5DB0E6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3A5BD9-4F1C-44F9-BDEA-8C1F442B7137}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44DCED42-2DE3-41DF-9BF8-CBCF7C2AF5A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2608,37 +2654,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3A5BD9-4F1C-44F9-BDEA-8C1F442B7137}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500F210C-5797-4401-A254-1609F5DB0E6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FDBEAEB-23AE-46E2-827B-BF6C7AC8C447}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7518fa5f-d3e5-45ff-bc46-9421360fd0ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="24e64fd7-dd82-45ab-bc56-7bee2b649a8c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>